<commit_message>
Started updating to 2022 data
</commit_message>
<xml_diff>
--- a/Tables/LFS_population_degurba.xlsx
+++ b/Tables/LFS_population_degurba.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:D203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -386,13 +386,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.4783687928924928</v>
+        <v>0.4801381671853858</v>
       </c>
       <c r="C2">
-        <v>0.2330458866351453</v>
+        <v>0.2375053055442568</v>
       </c>
       <c r="D2">
-        <v>0.2885853204723619</v>
+        <v>0.2823565272703574</v>
       </c>
     </row>
     <row r="3">
@@ -402,13 +402,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.2075865310689051</v>
+        <v>0.200019568689925</v>
       </c>
       <c r="C3">
-        <v>0.2616613201963621</v>
+        <v>0.2703241865716432</v>
       </c>
       <c r="D3">
-        <v>0.5307521487347328</v>
+        <v>0.5296562447384319</v>
       </c>
     </row>
     <row r="4">
@@ -418,13 +418,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.147638058902713</v>
+        <v>0.1470441402347462</v>
       </c>
       <c r="C4">
-        <v>0.4179864182563791</v>
+        <v>0.4158614279781007</v>
       </c>
       <c r="D4">
-        <v>0.434375522840908</v>
+        <v>0.4370944317871531</v>
       </c>
     </row>
     <row r="5">
@@ -444,13 +444,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.3225426975553784</v>
+        <v>0.3550323169830687</v>
       </c>
       <c r="C6">
-        <v>0.6605269992581927</v>
+        <v>0.6119450816683405</v>
       </c>
       <c r="D6">
-        <v>0.01693030318642889</v>
+        <v>0.03302260134859085</v>
       </c>
     </row>
     <row r="7">
@@ -460,10 +460,10 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.8527195865522995</v>
+        <v>0.8123341070165488</v>
       </c>
       <c r="D7">
-        <v>0.1472804134477005</v>
+        <v>0.1876658929834512</v>
       </c>
     </row>
     <row r="8">
@@ -473,13 +473,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.1589941718441562</v>
+        <v>0.1968168385449161</v>
       </c>
       <c r="C8">
-        <v>0.7500462970718756</v>
+        <v>0.7249546088762631</v>
       </c>
       <c r="D8">
-        <v>0.09095953108396818</v>
+        <v>0.07822855257882079</v>
       </c>
     </row>
     <row r="9">
@@ -489,13 +489,13 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.102827904268999</v>
+        <v>0.1069884915690053</v>
       </c>
       <c r="C9">
-        <v>0.7856342238263967</v>
+        <v>0.7694318950106976</v>
       </c>
       <c r="D9">
-        <v>0.1115378719046042</v>
+        <v>0.1235796134202971</v>
       </c>
     </row>
     <row r="10">
@@ -505,13 +505,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.2239684634952235</v>
+        <v>0.2301934206486993</v>
       </c>
       <c r="C10">
-        <v>0.606260184725002</v>
+        <v>0.5946201945360796</v>
       </c>
       <c r="D10">
-        <v>0.1697713517797746</v>
+        <v>0.175186384815221</v>
       </c>
     </row>
     <row r="11">
@@ -521,10 +521,10 @@
         </is>
       </c>
       <c r="C11">
-        <v>0.7887216560481126</v>
+        <v>0.8634588768770383</v>
       </c>
       <c r="D11">
-        <v>0.2112783439518874</v>
+        <v>0.1365411231229617</v>
       </c>
     </row>
     <row r="12">
@@ -534,13 +534,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.3244173042350813</v>
+        <v>0.4032454626513123</v>
       </c>
       <c r="C12">
-        <v>0.5279306604210996</v>
+        <v>0.4637618619991733</v>
       </c>
       <c r="D12">
-        <v>0.1476520353438191</v>
+        <v>0.1329926753495144</v>
       </c>
     </row>
     <row r="13">
@@ -550,13 +550,13 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.334978133577055</v>
+        <v>0.3807604279732316</v>
       </c>
       <c r="C13">
-        <v>0.4136407243011032</v>
+        <v>0.3783029615954263</v>
       </c>
       <c r="D13">
-        <v>0.2513811421218419</v>
+        <v>0.2409366104313421</v>
       </c>
     </row>
     <row r="14">
@@ -566,10 +566,10 @@
         </is>
       </c>
       <c r="C14">
-        <v>0.349823344312037</v>
+        <v>0.3233659260754168</v>
       </c>
       <c r="D14">
-        <v>0.650176655687963</v>
+        <v>0.6766340739245833</v>
       </c>
     </row>
     <row r="15">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.1992576893008621</v>
+        <v>0.2057723991013672</v>
       </c>
       <c r="C15">
-        <v>0.2782944330190206</v>
+        <v>0.25220810659941</v>
       </c>
       <c r="D15">
-        <v>0.5224478776801172</v>
+        <v>0.5420194942992228</v>
       </c>
     </row>
     <row r="16">
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.3241116793347238</v>
+        <v>0.3214238734442227</v>
       </c>
       <c r="C16">
-        <v>0.3269709022907596</v>
+        <v>0.3503126447582802</v>
       </c>
       <c r="D16">
-        <v>0.3489174183745166</v>
+        <v>0.3282634817974971</v>
       </c>
     </row>
     <row r="17">
@@ -611,13 +611,13 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.3215389647750784</v>
+        <v>0.2962338944465354</v>
       </c>
       <c r="C17">
-        <v>0.3526304803395588</v>
+        <v>0.3732008788470936</v>
       </c>
       <c r="D17">
-        <v>0.3258305548853628</v>
+        <v>0.330565226706371</v>
       </c>
     </row>
     <row r="18">
@@ -627,13 +627,13 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.5857987416352696</v>
+        <v>0.574977613713251</v>
       </c>
       <c r="C18">
-        <v>0.1751612691536163</v>
+        <v>0.1891670764116822</v>
       </c>
       <c r="D18">
-        <v>0.2390399892111141</v>
+        <v>0.2358553098750669</v>
       </c>
     </row>
     <row r="19">
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.5401788953310107</v>
+        <v>0.5505516730847339</v>
       </c>
       <c r="C19">
-        <v>0.1998850649479635</v>
+        <v>0.1991908091958023</v>
       </c>
       <c r="D19">
-        <v>0.2599360397210259</v>
+        <v>0.2502575177194638</v>
       </c>
     </row>
     <row r="20">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.6786461598137113</v>
+        <v>0.6856115303285418</v>
       </c>
       <c r="C20">
-        <v>0.1743467270296717</v>
+        <v>0.1704579852843193</v>
       </c>
       <c r="D20">
-        <v>0.147007113156617</v>
+        <v>0.143930484387139</v>
       </c>
     </row>
     <row r="21">
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.353450514371117</v>
+        <v>0.3614237743852208</v>
       </c>
       <c r="C21">
-        <v>0.3367688846390788</v>
+        <v>0.3356347630892328</v>
       </c>
       <c r="D21">
-        <v>0.3097806009898042</v>
+        <v>0.3029414625255464</v>
       </c>
     </row>
     <row r="22">
@@ -691,13 +691,13 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.5741373542165972</v>
+        <v>0.5268883943295189</v>
       </c>
       <c r="C22">
-        <v>0.2385035014669387</v>
+        <v>0.2907272495802266</v>
       </c>
       <c r="D22">
-        <v>0.1873591443164641</v>
+        <v>0.1823843560902544</v>
       </c>
     </row>
     <row r="23">
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.05019508212247041</v>
+        <v>0.05733582193303879</v>
       </c>
       <c r="C24">
-        <v>0.490652620847967</v>
+        <v>0.4902352033644323</v>
       </c>
       <c r="D24">
-        <v>0.4591522970295626</v>
+        <v>0.452428974702529</v>
       </c>
     </row>
     <row r="25">
@@ -733,13 +733,13 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.2228787687925225</v>
+        <v>0.2158837355968376</v>
       </c>
       <c r="C25">
-        <v>0.2903835484349147</v>
+        <v>0.3083599153999025</v>
       </c>
       <c r="D25">
-        <v>0.4867376827725629</v>
+        <v>0.4757563490032598</v>
       </c>
     </row>
     <row r="26">
@@ -749,13 +749,13 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.2405873106508891</v>
+        <v>0.2644248703421836</v>
       </c>
       <c r="C26">
-        <v>0.4780832832027875</v>
+        <v>0.466035544061475</v>
       </c>
       <c r="D26">
-        <v>0.2813294061463233</v>
+        <v>0.2695395855963414</v>
       </c>
     </row>
     <row r="27">
@@ -765,13 +765,13 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.1979172834303212</v>
+        <v>0.1944254363077888</v>
       </c>
       <c r="C27">
-        <v>0.3693607204931464</v>
+        <v>0.3644787067008379</v>
       </c>
       <c r="D27">
-        <v>0.4327219960765324</v>
+        <v>0.4410958569913733</v>
       </c>
     </row>
     <row r="28">
@@ -781,13 +781,13 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.261217832649573</v>
+        <v>0.2604861753813917</v>
       </c>
       <c r="C28">
-        <v>0.2862836106617093</v>
+        <v>0.2712944373050392</v>
       </c>
       <c r="D28">
-        <v>0.4524985566887177</v>
+        <v>0.4682193873135691</v>
       </c>
     </row>
     <row r="29">
@@ -797,13 +797,13 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.1452481751679376</v>
+        <v>0.1371392565147308</v>
       </c>
       <c r="C29">
-        <v>0.3904248785035349</v>
+        <v>0.4105077915754281</v>
       </c>
       <c r="D29">
-        <v>0.4643269463285274</v>
+        <v>0.4523529519098411</v>
       </c>
     </row>
     <row r="30">
@@ -813,13 +813,13 @@
         </is>
       </c>
       <c r="B30">
-        <v>0.3371329506339412</v>
+        <v>0.3355181174903821</v>
       </c>
       <c r="C30">
-        <v>0.4232590807179988</v>
+        <v>0.4323156086333569</v>
       </c>
       <c r="D30">
-        <v>0.23960796864806</v>
+        <v>0.232166273876261</v>
       </c>
     </row>
     <row r="31">
@@ -829,13 +829,13 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.2739245286641783</v>
+        <v>0.248627650066806</v>
       </c>
       <c r="C31">
-        <v>0.533008960144409</v>
+        <v>0.5497189304162232</v>
       </c>
       <c r="D31">
-        <v>0.1930665111914127</v>
+        <v>0.2016534195169708</v>
       </c>
     </row>
     <row r="32">
@@ -845,13 +845,13 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.2882453398814261</v>
+        <v>0.2737747589309151</v>
       </c>
       <c r="C32">
-        <v>0.3885114301851523</v>
+        <v>0.398996331957534</v>
       </c>
       <c r="D32">
-        <v>0.3232432299334216</v>
+        <v>0.3272289091115508</v>
       </c>
     </row>
     <row r="33">
@@ -871,13 +871,13 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.1775193468193179</v>
+        <v>0.1529994548309073</v>
       </c>
       <c r="C34">
-        <v>0.4977670956582491</v>
+        <v>0.4766107619861562</v>
       </c>
       <c r="D34">
-        <v>0.324713557522433</v>
+        <v>0.3703897831829365</v>
       </c>
     </row>
     <row r="35">
@@ -907,13 +907,13 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.3169041480325611</v>
+        <v>0.3051857079952445</v>
       </c>
       <c r="C37">
-        <v>0.5104104557183187</v>
+        <v>0.5115327151061652</v>
       </c>
       <c r="D37">
-        <v>0.1726853962491202</v>
+        <v>0.1832815768985903</v>
       </c>
     </row>
     <row r="38">
@@ -923,13 +923,13 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.2931005290887266</v>
+        <v>0.2995959895495935</v>
       </c>
       <c r="C38">
-        <v>0.240549572257732</v>
+        <v>0.230212136533016</v>
       </c>
       <c r="D38">
-        <v>0.4663498986535414</v>
+        <v>0.4701918739173904</v>
       </c>
     </row>
     <row r="39">
@@ -939,13 +939,13 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.2336468992534767</v>
+        <v>0.2291431781997648</v>
       </c>
       <c r="C39">
-        <v>0.4475042911695095</v>
+        <v>0.4203273151888832</v>
       </c>
       <c r="D39">
-        <v>0.3188488095770138</v>
+        <v>0.350529506611352</v>
       </c>
     </row>
     <row r="40">
@@ -955,13 +955,13 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.4994305759542673</v>
+        <v>0.4681083835506638</v>
       </c>
       <c r="C40">
-        <v>0.4159496566748256</v>
+        <v>0.4323553975264094</v>
       </c>
       <c r="D40">
-        <v>0.08461976737090708</v>
+        <v>0.09953621892292681</v>
       </c>
     </row>
     <row r="41">
@@ -971,13 +971,13 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.2053021194068032</v>
+        <v>0.2008109056717904</v>
       </c>
       <c r="C41">
-        <v>0.4478177700497177</v>
+        <v>0.4548070964662009</v>
       </c>
       <c r="D41">
-        <v>0.3468801105434791</v>
+        <v>0.3443819978620086</v>
       </c>
     </row>
     <row r="42">
@@ -987,13 +987,13 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.1580397492916122</v>
+        <v>0.1697447043138994</v>
       </c>
       <c r="C42">
-        <v>0.6937820912614832</v>
+        <v>0.6641875781335427</v>
       </c>
       <c r="D42">
-        <v>0.1481781594469047</v>
+        <v>0.1660677175525579</v>
       </c>
     </row>
     <row r="43">
@@ -1003,13 +1003,13 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.4097792740475261</v>
+        <v>0.4014335894495782</v>
       </c>
       <c r="C43">
-        <v>0.3763441492288278</v>
+        <v>0.3796872685681998</v>
       </c>
       <c r="D43">
-        <v>0.213876576723646</v>
+        <v>0.2188791419822219</v>
       </c>
     </row>
     <row r="44">
@@ -1019,13 +1019,13 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.2513264278307353</v>
+        <v>0.251828318883488</v>
       </c>
       <c r="C44">
-        <v>0.3467321453698567</v>
+        <v>0.3230965058477213</v>
       </c>
       <c r="D44">
-        <v>0.401941426799408</v>
+        <v>0.4250751752687907</v>
       </c>
     </row>
     <row r="45">
@@ -1035,13 +1035,13 @@
         </is>
       </c>
       <c r="B45">
-        <v>0.2544473237443898</v>
+        <v>0.2188512196247723</v>
       </c>
       <c r="C45">
-        <v>0.4384140699022602</v>
+        <v>0.4786067494448314</v>
       </c>
       <c r="D45">
-        <v>0.3071386063533499</v>
+        <v>0.3025420309303962</v>
       </c>
     </row>
     <row r="46">
@@ -1051,13 +1051,13 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.2335111731656943</v>
+        <v>0.2295001232641331</v>
       </c>
       <c r="C46">
-        <v>0.38008414905921</v>
+        <v>0.3527583594816675</v>
       </c>
       <c r="D46">
-        <v>0.3864046777750957</v>
+        <v>0.4177415172541994</v>
       </c>
     </row>
     <row r="47">
@@ -1067,13 +1067,13 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.6993617308754104</v>
+        <v>0.6957481983450137</v>
       </c>
       <c r="C47">
-        <v>0.2233021321932197</v>
+        <v>0.2263055187851367</v>
       </c>
       <c r="D47">
-        <v>0.07733613693136983</v>
+        <v>0.07794628286984961</v>
       </c>
     </row>
     <row r="48">
@@ -1083,13 +1083,13 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.0261430403617472</v>
+        <v>0.03004982405501126</v>
       </c>
       <c r="C48">
-        <v>0.4383923588651887</v>
+        <v>0.451161727844135</v>
       </c>
       <c r="D48">
-        <v>0.5354646007730641</v>
+        <v>0.5187884481008538</v>
       </c>
     </row>
     <row r="49">
@@ -1099,13 +1099,13 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.1624105794773607</v>
+        <v>0.1595676432324896</v>
       </c>
       <c r="C49">
-        <v>0.3380275295747839</v>
+        <v>0.3369102188160465</v>
       </c>
       <c r="D49">
-        <v>0.4995618909478554</v>
+        <v>0.5035221379514638</v>
       </c>
     </row>
     <row r="50">
@@ -1115,13 +1115,13 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.2567233458837264</v>
+        <v>0.2575504325657641</v>
       </c>
       <c r="C50">
-        <v>0.2412809447919854</v>
+        <v>0.2460875498523071</v>
       </c>
       <c r="D50">
-        <v>0.5019957093242882</v>
+        <v>0.4963620175819288</v>
       </c>
     </row>
     <row r="51">
@@ -1131,13 +1131,13 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.2147531228906401</v>
+        <v>0.241250731458918</v>
       </c>
       <c r="C51">
-        <v>0.190700154364865</v>
+        <v>0.1649125719677216</v>
       </c>
       <c r="D51">
-        <v>0.5945467227444949</v>
+        <v>0.5938366965733605</v>
       </c>
     </row>
     <row r="52">
@@ -1147,13 +1147,13 @@
         </is>
       </c>
       <c r="B52">
-        <v>0.468547600779376</v>
+        <v>0.4752029807197243</v>
       </c>
       <c r="C52">
-        <v>0.1841388752769974</v>
+        <v>0.1871094257185379</v>
       </c>
       <c r="D52">
-        <v>0.3473135239436266</v>
+        <v>0.3376875935617378</v>
       </c>
     </row>
     <row r="53">
@@ -1163,13 +1163,13 @@
         </is>
       </c>
       <c r="B53">
-        <v>0.655082332675802</v>
+        <v>0.6492413263223674</v>
       </c>
       <c r="C53">
-        <v>0.3171810127739268</v>
+        <v>0.3156733962492812</v>
       </c>
       <c r="D53">
-        <v>0.02773665455027122</v>
+        <v>0.03508527742835137</v>
       </c>
     </row>
     <row r="54">
@@ -1179,10 +1179,10 @@
         </is>
       </c>
       <c r="C54">
-        <v>0.4683096512414137</v>
+        <v>0.4762562106657975</v>
       </c>
       <c r="D54">
-        <v>0.5316903487585863</v>
+        <v>0.5237437893342025</v>
       </c>
     </row>
     <row r="55">
@@ -1192,13 +1192,13 @@
         </is>
       </c>
       <c r="B55">
-        <v>0.2257977819725625</v>
+        <v>0.2407480354976044</v>
       </c>
       <c r="C55">
-        <v>0.282480768827335</v>
+        <v>0.2770808381941803</v>
       </c>
       <c r="D55">
-        <v>0.4917214492001025</v>
+        <v>0.4821711263082153</v>
       </c>
     </row>
     <row r="56">
@@ -1208,13 +1208,13 @@
         </is>
       </c>
       <c r="B56">
-        <v>0.3457120995551571</v>
+        <v>0.3302685840370821</v>
       </c>
       <c r="C56">
-        <v>0.2219641241176648</v>
+        <v>0.2236597331728754</v>
       </c>
       <c r="D56">
-        <v>0.4323237763271781</v>
+        <v>0.4460716827900426</v>
       </c>
     </row>
     <row r="57">
@@ -1224,13 +1224,13 @@
         </is>
       </c>
       <c r="B57">
-        <v>0.08635190421137261</v>
+        <v>0.09906750052256103</v>
       </c>
       <c r="C57">
-        <v>0.5050413020909337</v>
+        <v>0.5107487928301049</v>
       </c>
       <c r="D57">
-        <v>0.4086067936976937</v>
+        <v>0.3901837066473341</v>
       </c>
     </row>
     <row r="58">
@@ -1240,13 +1240,13 @@
         </is>
       </c>
       <c r="B58">
-        <v>0.3407881936881014</v>
+        <v>0.351408858351164</v>
       </c>
       <c r="C58">
-        <v>0.3869321259884556</v>
+        <v>0.3785527429757538</v>
       </c>
       <c r="D58">
-        <v>0.272279680323443</v>
+        <v>0.2700383986730823</v>
       </c>
     </row>
     <row r="59">
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C59">
-        <v>0.5963138625362624</v>
+        <v>0.5660752163959423</v>
       </c>
       <c r="D59">
-        <v>0.4036861374637375</v>
+        <v>0.4339247836040577</v>
       </c>
     </row>
     <row r="60">
@@ -1269,13 +1269,13 @@
         </is>
       </c>
       <c r="B60">
-        <v>0.2541151495552224</v>
+        <v>0.2657191866174279</v>
       </c>
       <c r="C60">
-        <v>0.2310344101986336</v>
+        <v>0.2429025472453399</v>
       </c>
       <c r="D60">
-        <v>0.514850440246144</v>
+        <v>0.4913782661372322</v>
       </c>
     </row>
     <row r="61">
@@ -1285,13 +1285,13 @@
         </is>
       </c>
       <c r="B61">
-        <v>0.4756213209341338</v>
+        <v>0.4713843032886761</v>
       </c>
       <c r="C61">
-        <v>0.2248214260953872</v>
+        <v>0.1965997294242002</v>
       </c>
       <c r="D61">
-        <v>0.299557252970479</v>
+        <v>0.3320159672871236</v>
       </c>
     </row>
     <row r="62">
@@ -1301,10 +1301,10 @@
         </is>
       </c>
       <c r="C62">
-        <v>0.3167922605569926</v>
+        <v>0.352248621600596</v>
       </c>
       <c r="D62">
-        <v>0.6832077394430074</v>
+        <v>0.647751378399404</v>
       </c>
     </row>
     <row r="63">
@@ -1314,13 +1314,13 @@
         </is>
       </c>
       <c r="B63">
-        <v>0.235444863869637</v>
+        <v>0.2190164095055936</v>
       </c>
       <c r="C63">
-        <v>0.2885899198607457</v>
+        <v>0.2873777764971092</v>
       </c>
       <c r="D63">
-        <v>0.4759652162696173</v>
+        <v>0.4936058139972972</v>
       </c>
     </row>
     <row r="64">
@@ -1330,13 +1330,13 @@
         </is>
       </c>
       <c r="B64">
-        <v>0.1118245973435775</v>
+        <v>0.1220838289291086</v>
       </c>
       <c r="C64">
-        <v>0.3518482440476635</v>
+        <v>0.3677067277991732</v>
       </c>
       <c r="D64">
-        <v>0.5363271586087591</v>
+        <v>0.5102094432717182</v>
       </c>
     </row>
     <row r="65">
@@ -1346,13 +1346,13 @@
         </is>
       </c>
       <c r="B65">
-        <v>0.142139826257551</v>
+        <v>0.1437986199634324</v>
       </c>
       <c r="C65">
-        <v>0.341752899889342</v>
+        <v>0.3540268814683065</v>
       </c>
       <c r="D65">
-        <v>0.516107273853107</v>
+        <v>0.5021744985682612</v>
       </c>
     </row>
     <row r="66">
@@ -1362,13 +1362,13 @@
         </is>
       </c>
       <c r="B66">
-        <v>0.3940602378837285</v>
+        <v>0.3923840160173315</v>
       </c>
       <c r="C66">
-        <v>0.3831701336589442</v>
+        <v>0.3858674132416352</v>
       </c>
       <c r="D66">
-        <v>0.2227696284573273</v>
+        <v>0.2217485707410333</v>
       </c>
     </row>
     <row r="67">
@@ -1378,13 +1378,13 @@
         </is>
       </c>
       <c r="B67">
-        <v>0.5828735598218029</v>
+        <v>0.6095798674465184</v>
       </c>
       <c r="C67">
-        <v>0.2652540053221826</v>
+        <v>0.2217929072546157</v>
       </c>
       <c r="D67">
-        <v>0.1518724348560145</v>
+        <v>0.168627225298866</v>
       </c>
     </row>
     <row r="68">
@@ -1394,13 +1394,13 @@
         </is>
       </c>
       <c r="B68">
-        <v>0.3676142900504177</v>
+        <v>0.3635983905841419</v>
       </c>
       <c r="C68">
-        <v>0.4060472764711747</v>
+        <v>0.4410951037558058</v>
       </c>
       <c r="D68">
-        <v>0.2263384334784076</v>
+        <v>0.1953065056600523</v>
       </c>
     </row>
     <row r="69">
@@ -1410,13 +1410,13 @@
         </is>
       </c>
       <c r="B69">
-        <v>0.5843379704681247</v>
+        <v>0.5959894197089494</v>
       </c>
       <c r="C69">
-        <v>0.2996569770952287</v>
+        <v>0.3040995465395913</v>
       </c>
       <c r="D69">
-        <v>0.1160050524366465</v>
+        <v>0.09991103375145934</v>
       </c>
     </row>
     <row r="70">
@@ -1426,13 +1426,13 @@
         </is>
       </c>
       <c r="B70">
-        <v>0.5287575088610843</v>
+        <v>0.5446753448179408</v>
       </c>
       <c r="C70">
-        <v>0.1559173097277941</v>
+        <v>0.1383131963175542</v>
       </c>
       <c r="D70">
-        <v>0.3153251814111217</v>
+        <v>0.3170114588645049</v>
       </c>
     </row>
     <row r="71">
@@ -1442,13 +1442,13 @@
         </is>
       </c>
       <c r="B71">
-        <v>0.451041905717392</v>
+        <v>0.4375906683613121</v>
       </c>
       <c r="C71">
-        <v>0.3174236553240745</v>
+        <v>0.3220267329934494</v>
       </c>
       <c r="D71">
-        <v>0.2315344389585335</v>
+        <v>0.2403825986452385</v>
       </c>
     </row>
     <row r="72">
@@ -1458,13 +1458,13 @@
         </is>
       </c>
       <c r="B72">
-        <v>0.5166998759259693</v>
+        <v>0.5128308336153844</v>
       </c>
       <c r="C72">
-        <v>0.2756638670363163</v>
+        <v>0.2854907550027662</v>
       </c>
       <c r="D72">
-        <v>0.2076362570377144</v>
+        <v>0.2016784113818495</v>
       </c>
     </row>
     <row r="73">
@@ -1474,13 +1474,13 @@
         </is>
       </c>
       <c r="B73">
-        <v>0.8107441206475552</v>
+        <v>0.7967132044580194</v>
       </c>
       <c r="C73">
-        <v>0.1662133928817123</v>
+        <v>0.1731322960419129</v>
       </c>
       <c r="D73">
-        <v>0.02304248647073252</v>
+        <v>0.03015449950006768</v>
       </c>
     </row>
     <row r="74">
@@ -1490,13 +1490,13 @@
         </is>
       </c>
       <c r="B74">
-        <v>0.4264656666375634</v>
+        <v>0.4274183813357549</v>
       </c>
       <c r="C74">
-        <v>0.2515775833331985</v>
+        <v>0.2403527586383244</v>
       </c>
       <c r="D74">
-        <v>0.3219567500292381</v>
+        <v>0.3322288600259207</v>
       </c>
     </row>
     <row r="75">
@@ -1506,13 +1506,13 @@
         </is>
       </c>
       <c r="B75">
-        <v>0.2883586561594272</v>
+        <v>0.2975360068755166</v>
       </c>
       <c r="C75">
-        <v>0.4436822015955895</v>
+        <v>0.4294863259275505</v>
       </c>
       <c r="D75">
-        <v>0.2679591422449833</v>
+        <v>0.2729776671969329</v>
       </c>
     </row>
     <row r="76">
@@ -1522,13 +1522,13 @@
         </is>
       </c>
       <c r="B76">
-        <v>0.3189027516166359</v>
+        <v>0.2966954138033222</v>
       </c>
       <c r="C76">
-        <v>0.3874579637190098</v>
+        <v>0.4266670666057706</v>
       </c>
       <c r="D76">
-        <v>0.2936392846643543</v>
+        <v>0.2766375195909071</v>
       </c>
     </row>
     <row r="77">
@@ -1538,13 +1538,13 @@
         </is>
       </c>
       <c r="B77">
-        <v>0.5975174589786867</v>
+        <v>0.5953840792812911</v>
       </c>
       <c r="C77">
-        <v>0.3013103040618447</v>
+        <v>0.3033337635273148</v>
       </c>
       <c r="D77">
-        <v>0.1011722369594686</v>
+        <v>0.101282157191394</v>
       </c>
     </row>
     <row r="78">
@@ -1554,13 +1554,13 @@
         </is>
       </c>
       <c r="B78">
-        <v>0.4931049249199718</v>
+        <v>0.518508171990409</v>
       </c>
       <c r="C78">
-        <v>0.4239027835315228</v>
+        <v>0.3930652320982334</v>
       </c>
       <c r="D78">
-        <v>0.08299229154850542</v>
+        <v>0.08842659591135767</v>
       </c>
     </row>
     <row r="79">
@@ -1570,13 +1570,13 @@
         </is>
       </c>
       <c r="B79">
-        <v>0.4070190495080072</v>
+        <v>0.4081095956145336</v>
       </c>
       <c r="C79">
-        <v>0.4662803800957144</v>
+        <v>0.4777953611509427</v>
       </c>
       <c r="D79">
-        <v>0.1267005703962785</v>
+        <v>0.1140950432345236</v>
       </c>
     </row>
     <row r="80">
@@ -1586,13 +1586,13 @@
         </is>
       </c>
       <c r="B80">
-        <v>0.5007861895679793</v>
+        <v>0.5259480128395304</v>
       </c>
       <c r="C80">
-        <v>0.3870777308597939</v>
+        <v>0.3605212783938843</v>
       </c>
       <c r="D80">
-        <v>0.1121360795722269</v>
+        <v>0.1135307087665853</v>
       </c>
     </row>
     <row r="81">
@@ -1602,13 +1602,10 @@
         </is>
       </c>
       <c r="B81">
-        <v>0.5089825333833888</v>
+        <v>0.5154448546644527</v>
       </c>
       <c r="C81">
-        <v>0.4815646457966291</v>
-      </c>
-      <c r="D81">
-        <v>0.009452820819982157</v>
+        <v>0.4845551453355473</v>
       </c>
     </row>
     <row r="82">
@@ -1638,13 +1635,13 @@
         </is>
       </c>
       <c r="B84">
-        <v>0.4597677059483186</v>
+        <v>0.4102531469225507</v>
       </c>
       <c r="C84">
-        <v>0.5007423281358631</v>
+        <v>0.553340603982824</v>
       </c>
       <c r="D84">
-        <v>0.03948996591581843</v>
+        <v>0.03640624909462524</v>
       </c>
     </row>
     <row r="85">
@@ -1654,13 +1651,13 @@
         </is>
       </c>
       <c r="B85">
-        <v>0.2848646751337644</v>
+        <v>0.2896233041236547</v>
       </c>
       <c r="C85">
-        <v>0.3193274686662168</v>
+        <v>0.3097598213584447</v>
       </c>
       <c r="D85">
-        <v>0.3958078562000188</v>
+        <v>0.4006168745179007</v>
       </c>
     </row>
     <row r="86">
@@ -1670,13 +1667,13 @@
         </is>
       </c>
       <c r="B86">
-        <v>0.7185417205363842</v>
+        <v>0.7163043818898654</v>
       </c>
       <c r="C86">
-        <v>0.1652698573842291</v>
+        <v>0.1637473956590144</v>
       </c>
       <c r="D86">
-        <v>0.1161884220793867</v>
+        <v>0.1199482224511201</v>
       </c>
     </row>
     <row r="87">
@@ -1686,13 +1683,13 @@
         </is>
       </c>
       <c r="B87">
-        <v>0.2701420428606425</v>
+        <v>0.2602151199329291</v>
       </c>
       <c r="C87">
-        <v>0.4711970082123263</v>
+        <v>0.4421537156449524</v>
       </c>
       <c r="D87">
-        <v>0.2586609489270312</v>
+        <v>0.2976311644221185</v>
       </c>
     </row>
     <row r="88">
@@ -1702,13 +1699,13 @@
         </is>
       </c>
       <c r="B88">
-        <v>0.2708300490007869</v>
+        <v>0.2747558809016778</v>
       </c>
       <c r="C88">
-        <v>0.3613859553375946</v>
+        <v>0.3555844872120477</v>
       </c>
       <c r="D88">
-        <v>0.3677839956616185</v>
+        <v>0.3696596318862745</v>
       </c>
     </row>
     <row r="89">
@@ -1718,10 +1715,10 @@
         </is>
       </c>
       <c r="C89">
-        <v>0.3736381724819609</v>
+        <v>0.3308895038985798</v>
       </c>
       <c r="D89">
-        <v>0.6263618275180391</v>
+        <v>0.6691104961014201</v>
       </c>
     </row>
     <row r="90">
@@ -1731,13 +1728,13 @@
         </is>
       </c>
       <c r="B90">
-        <v>0.818258324199949</v>
+        <v>0.82919326613677</v>
       </c>
       <c r="C90">
-        <v>0.129324664316264</v>
+        <v>0.1116906074230279</v>
       </c>
       <c r="D90">
-        <v>0.052417011483787</v>
+        <v>0.059116126440202</v>
       </c>
     </row>
     <row r="91">
@@ -1747,13 +1744,13 @@
         </is>
       </c>
       <c r="B91">
-        <v>0.2869597490483223</v>
+        <v>0.2880721149280791</v>
       </c>
       <c r="C91">
-        <v>0.2036243209378868</v>
+        <v>0.1692150376661829</v>
       </c>
       <c r="D91">
-        <v>0.5094159300137909</v>
+        <v>0.542712847405738</v>
       </c>
     </row>
     <row r="92">
@@ -1763,13 +1760,13 @@
         </is>
       </c>
       <c r="B92">
-        <v>0.2211723319532488</v>
+        <v>0.2486489935366317</v>
       </c>
       <c r="C92">
-        <v>0.2312306011516097</v>
+        <v>0.1926832811677678</v>
       </c>
       <c r="D92">
-        <v>0.5475970668951414</v>
+        <v>0.5586677252956005</v>
       </c>
     </row>
     <row r="93">
@@ -1779,13 +1776,13 @@
         </is>
       </c>
       <c r="B93">
-        <v>0.2921974874752201</v>
+        <v>0.2012074222493638</v>
       </c>
       <c r="C93">
-        <v>0.1159106588919604</v>
+        <v>0.1322854944299177</v>
       </c>
       <c r="D93">
-        <v>0.5918918536328195</v>
+        <v>0.6665070833207185</v>
       </c>
     </row>
     <row r="94">
@@ -1795,13 +1792,13 @@
         </is>
       </c>
       <c r="B94">
-        <v>0.2654760761074836</v>
+        <v>0.1582206632448353</v>
       </c>
       <c r="C94">
-        <v>0.1981411779524491</v>
+        <v>0.2162604149025897</v>
       </c>
       <c r="D94">
-        <v>0.5363827459400673</v>
+        <v>0.625518921852575</v>
       </c>
     </row>
     <row r="95">
@@ -1811,13 +1808,13 @@
         </is>
       </c>
       <c r="B95">
-        <v>0.3799843707203666</v>
+        <v>0.3339833795109498</v>
       </c>
       <c r="C95">
-        <v>0.1560766138495114</v>
+        <v>0.2725898284600738</v>
       </c>
       <c r="D95">
-        <v>0.4639390154301221</v>
+        <v>0.3934267920289763</v>
       </c>
     </row>
     <row r="96">
@@ -1827,13 +1824,13 @@
         </is>
       </c>
       <c r="B96">
-        <v>0.5587037535118738</v>
+        <v>0.5663172097515013</v>
       </c>
       <c r="C96">
-        <v>0.2313455174330026</v>
+        <v>0.1925460408369052</v>
       </c>
       <c r="D96">
-        <v>0.2099507290551236</v>
+        <v>0.2411367494115934</v>
       </c>
     </row>
     <row r="97">
@@ -1843,13 +1840,13 @@
         </is>
       </c>
       <c r="B97">
-        <v>0.188461422736157</v>
+        <v>0.2345866460059325</v>
       </c>
       <c r="C97">
-        <v>0.2698705609957958</v>
+        <v>0.2402952215365823</v>
       </c>
       <c r="D97">
-        <v>0.5416680162680473</v>
+        <v>0.5251181324574852</v>
       </c>
     </row>
     <row r="98">
@@ -1859,13 +1856,13 @@
         </is>
       </c>
       <c r="B98">
-        <v>0.3676260486046784</v>
+        <v>0.2915746086630191</v>
       </c>
       <c r="C98">
-        <v>0.308699329591046</v>
+        <v>0.3588248660251951</v>
       </c>
       <c r="D98">
-        <v>0.3236746218042756</v>
+        <v>0.3496005253117858</v>
       </c>
     </row>
     <row r="99">
@@ -1875,13 +1872,13 @@
         </is>
       </c>
       <c r="B99">
-        <v>0.3048803951529663</v>
+        <v>0.2573567710340315</v>
       </c>
       <c r="C99">
-        <v>0.1885902118947553</v>
+        <v>0.1589375853256542</v>
       </c>
       <c r="D99">
-        <v>0.5065293929522784</v>
+        <v>0.5837056436403143</v>
       </c>
     </row>
     <row r="100">
@@ -1891,13 +1888,13 @@
         </is>
       </c>
       <c r="B100">
-        <v>0.1983829679024585</v>
+        <v>0.228799815133177</v>
       </c>
       <c r="C100">
-        <v>0.4139226391939069</v>
+        <v>0.3822945918699104</v>
       </c>
       <c r="D100">
-        <v>0.3876943929036347</v>
+        <v>0.3889055929969126</v>
       </c>
     </row>
     <row r="101">
@@ -1907,13 +1904,13 @@
         </is>
       </c>
       <c r="B101">
-        <v>0.3463859869385996</v>
+        <v>0.362815306114001</v>
       </c>
       <c r="C101">
-        <v>0.1209426592504056</v>
+        <v>0.09380080649042789</v>
       </c>
       <c r="D101">
-        <v>0.5326713538109947</v>
+        <v>0.5433838873955711</v>
       </c>
     </row>
     <row r="102">
@@ -1923,13 +1920,13 @@
         </is>
       </c>
       <c r="B102">
-        <v>0.3157651378090066</v>
+        <v>0.3610098386966902</v>
       </c>
       <c r="C102">
-        <v>0.1687124896780295</v>
+        <v>0.1582441031819359</v>
       </c>
       <c r="D102">
-        <v>0.515522372512964</v>
+        <v>0.4807460581213739</v>
       </c>
     </row>
     <row r="103">
@@ -1939,13 +1936,13 @@
         </is>
       </c>
       <c r="B103">
-        <v>0.2906232804720537</v>
+        <v>0.3084235163894465</v>
       </c>
       <c r="C103">
-        <v>0.1697591250028058</v>
+        <v>0.1353747561819083</v>
       </c>
       <c r="D103">
-        <v>0.5396175945251405</v>
+        <v>0.5562017274286453</v>
       </c>
     </row>
     <row r="104">
@@ -1955,13 +1952,13 @@
         </is>
       </c>
       <c r="B104">
-        <v>0.3138760604926678</v>
+        <v>0.2808458302141685</v>
       </c>
       <c r="C104">
-        <v>0.07629239210291726</v>
+        <v>0.08033412239758377</v>
       </c>
       <c r="D104">
-        <v>0.6098315474044149</v>
+        <v>0.6388200473882477</v>
       </c>
     </row>
     <row r="105">
@@ -1971,13 +1968,13 @@
         </is>
       </c>
       <c r="B105">
-        <v>0.2659688620856317</v>
+        <v>0.1953401770793518</v>
       </c>
       <c r="C105">
-        <v>0.1018145265542447</v>
+        <v>0.110665014085015</v>
       </c>
       <c r="D105">
-        <v>0.6322166113601236</v>
+        <v>0.6939948088356332</v>
       </c>
     </row>
     <row r="106">
@@ -1987,13 +1984,13 @@
         </is>
       </c>
       <c r="B106">
-        <v>0.3812075720724816</v>
+        <v>0.3570994617896079</v>
       </c>
       <c r="C106">
-        <v>0.2399069153105613</v>
+        <v>0.2928966059074237</v>
       </c>
       <c r="D106">
-        <v>0.3788855126169571</v>
+        <v>0.3500039323029684</v>
       </c>
     </row>
     <row r="107">
@@ -2003,13 +2000,13 @@
         </is>
       </c>
       <c r="B107">
-        <v>0.334483956863093</v>
+        <v>0.3569525783300787</v>
       </c>
       <c r="C107">
-        <v>0.2542139277780268</v>
+        <v>0.2154057807448895</v>
       </c>
       <c r="D107">
-        <v>0.4113021153588802</v>
+        <v>0.4276416409250318</v>
       </c>
     </row>
     <row r="108">
@@ -2019,13 +2016,13 @@
         </is>
       </c>
       <c r="B108">
-        <v>0.2003880431743607</v>
+        <v>0.2411218345865961</v>
       </c>
       <c r="C108">
-        <v>0.1563860801470402</v>
+        <v>0.1494817293360517</v>
       </c>
       <c r="D108">
-        <v>0.6432258766785991</v>
+        <v>0.6093964360773522</v>
       </c>
     </row>
     <row r="109">
@@ -2035,13 +2032,13 @@
         </is>
       </c>
       <c r="B109">
-        <v>0.3310028019026077</v>
+        <v>0.2733178436085252</v>
       </c>
       <c r="C109">
-        <v>0.3367075249897259</v>
+        <v>0.3987890236190011</v>
       </c>
       <c r="D109">
-        <v>0.3322896731076663</v>
+        <v>0.3278931327724736</v>
       </c>
     </row>
     <row r="110">
@@ -2051,13 +2048,13 @@
         </is>
       </c>
       <c r="B110">
-        <v>0.6719232928538421</v>
+        <v>0.7128906274494481</v>
       </c>
       <c r="C110">
-        <v>0.1946013272601038</v>
+        <v>0.1476578426748319</v>
       </c>
       <c r="D110">
-        <v>0.1334753798860541</v>
+        <v>0.13945152987572</v>
       </c>
     </row>
     <row r="111">
@@ -2067,13 +2064,13 @@
         </is>
       </c>
       <c r="B111">
-        <v>0.3968194613348389</v>
+        <v>0.445986599731125</v>
       </c>
       <c r="C111">
-        <v>0.2146215696373621</v>
+        <v>0.1378597779565955</v>
       </c>
       <c r="D111">
-        <v>0.388558969027799</v>
+        <v>0.4161536223122795</v>
       </c>
     </row>
     <row r="112">
@@ -2093,10 +2090,10 @@
         </is>
       </c>
       <c r="B113">
-        <v>0.4197069064148882</v>
+        <v>0.394206524324107</v>
       </c>
       <c r="D113">
-        <v>0.5802930935851118</v>
+        <v>0.605793475675893</v>
       </c>
     </row>
     <row r="114">
@@ -2116,10 +2113,10 @@
         </is>
       </c>
       <c r="B115">
-        <v>0.2473604516999582</v>
+        <v>0.2756424298649358</v>
       </c>
       <c r="D115">
-        <v>0.7526395483000418</v>
+        <v>0.7243575701350642</v>
       </c>
     </row>
     <row r="116">
@@ -2129,13 +2126,13 @@
         </is>
       </c>
       <c r="B116">
-        <v>0.1217749095944155</v>
+        <v>0.1143724560249627</v>
       </c>
       <c r="C116">
-        <v>0.4268167356952102</v>
+        <v>0.4351732278104615</v>
       </c>
       <c r="D116">
-        <v>0.4514083547103743</v>
+        <v>0.4504543161645758</v>
       </c>
     </row>
     <row r="117">
@@ -2145,1381 +2142,1365 @@
         </is>
       </c>
       <c r="B117">
-        <v>0.2625164030915865</v>
+        <v>0.254590772933227</v>
       </c>
       <c r="C117">
-        <v>0.3438049078507825</v>
+        <v>0.3387325935246692</v>
       </c>
       <c r="D117">
-        <v>0.393678689057631</v>
+        <v>0.4066766335421039</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>HR04_Kontinentalna Hrvatska (old)</t>
+          <t>HR05_Grad Zagreb</t>
         </is>
       </c>
       <c r="B118">
-        <v>0.3696164624332907</v>
-      </c>
-      <c r="C118">
-        <v>0.288018340119548</v>
-      </c>
-      <c r="D118">
-        <v>0.3423651974471613</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>HR05_Grad Zagreb</t>
-        </is>
-      </c>
-      <c r="B119">
-        <v>1</v>
+          <t>HR06_Sjeverna Hrvatska</t>
+        </is>
+      </c>
+      <c r="C119">
+        <v>0.4576540078833723</v>
+      </c>
+      <c r="D119">
+        <v>0.5423459921166277</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>HR06_Sjeverna Hrvatska</t>
-        </is>
-      </c>
-      <c r="C120">
-        <v>0.4184175479122184</v>
-      </c>
-      <c r="D120">
-        <v>0.5815824520877816</v>
+          <t>HU11_Budapest</t>
+        </is>
+      </c>
+      <c r="B120">
+        <v>1</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>HU11_Budapest</t>
-        </is>
-      </c>
-      <c r="B121">
-        <v>1</v>
+          <t>HU12_Pest</t>
+        </is>
+      </c>
+      <c r="C121">
+        <v>0.8454212523501533</v>
+      </c>
+      <c r="D121">
+        <v>0.1545787476498466</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>HU12_Pest</t>
-        </is>
+          <t>HU21_Közép-Dunántúl</t>
+        </is>
+      </c>
+      <c r="B122">
+        <v>0.2061922069521274</v>
       </c>
       <c r="C122">
-        <v>0.8525162230663108</v>
+        <v>0.3645373214714938</v>
       </c>
       <c r="D122">
-        <v>0.1474837769336892</v>
+        <v>0.4292704715763788</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>HU21_Közép-Dunántúl</t>
+          <t>HU22_Nyugat-Dunántúl</t>
         </is>
       </c>
       <c r="B123">
-        <v>0.209468790466203</v>
+        <v>0.2174773467714825</v>
       </c>
       <c r="C123">
-        <v>0.3590907909928537</v>
+        <v>0.3243612826668297</v>
       </c>
       <c r="D123">
-        <v>0.4314404185409433</v>
+        <v>0.4581613705616878</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>HU22_Nyugat-Dunántúl</t>
+          <t>HU23_Dél-Dunántúl</t>
         </is>
       </c>
       <c r="B124">
-        <v>0.2205558138014013</v>
+        <v>0.1696782117082209</v>
       </c>
       <c r="C124">
-        <v>0.3248396602647431</v>
+        <v>0.2955214430443412</v>
       </c>
       <c r="D124">
-        <v>0.4546045259338556</v>
+        <v>0.5348003452474379</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>HU23_Dél-Dunántúl</t>
+          <t>HU31_Észak-Magyarország</t>
         </is>
       </c>
       <c r="B125">
-        <v>0.1642495920368739</v>
+        <v>0.1278238794026748</v>
       </c>
       <c r="C125">
-        <v>0.2959379315454284</v>
+        <v>0.3985285200114087</v>
       </c>
       <c r="D125">
-        <v>0.5398124764176977</v>
+        <v>0.4736476005859165</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>HU31_Észak-Magyarország</t>
+          <t>HU32_Észak-Alföld</t>
         </is>
       </c>
       <c r="B126">
-        <v>0.1246296778015987</v>
+        <v>0.2786825880366464</v>
       </c>
       <c r="C126">
-        <v>0.394631985714475</v>
+        <v>0.3692712307689576</v>
       </c>
       <c r="D126">
-        <v>0.4807383364839263</v>
+        <v>0.3520461811943961</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>HU32_Észak-Alföld</t>
+          <t>HU33_Dél-Alföld</t>
         </is>
       </c>
       <c r="B127">
-        <v>0.278168482837418</v>
+        <v>0.2136509390832828</v>
       </c>
       <c r="C127">
-        <v>0.376482733443172</v>
+        <v>0.4221767533105455</v>
       </c>
       <c r="D127">
-        <v>0.34534878371941</v>
+        <v>0.3641723076061718</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>HU33_Dél-Alföld</t>
+          <t>IE04_Northern and Western</t>
         </is>
       </c>
       <c r="B128">
-        <v>0.2075724706897875</v>
+        <v>0.1172670058114021</v>
       </c>
       <c r="C128">
-        <v>0.4314506348346226</v>
+        <v>0.117978892603331</v>
       </c>
       <c r="D128">
-        <v>0.3609768944755898</v>
+        <v>0.7647541015852669</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>IE04_Northern and Western</t>
+          <t>IE05_Southern</t>
         </is>
       </c>
       <c r="B129">
-        <v>0.1135933185310228</v>
+        <v>0.1388392489774525</v>
       </c>
       <c r="C129">
-        <v>0.1150802823088337</v>
+        <v>0.3117966796003005</v>
       </c>
       <c r="D129">
-        <v>0.7713263991601434</v>
+        <v>0.549364071422247</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>IE05_Southern</t>
+          <t>IE06_Eastern and Midland</t>
         </is>
       </c>
       <c r="B130">
-        <v>0.1352263828963648</v>
+        <v>0.603533782383867</v>
       </c>
       <c r="C130">
-        <v>0.3094416887834672</v>
+        <v>0.2035030419240041</v>
       </c>
       <c r="D130">
-        <v>0.555331928320168</v>
+        <v>0.1929631756921288</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>IE06_Eastern and Midland</t>
+          <t>ITC1_Piemonte</t>
         </is>
       </c>
       <c r="B131">
-        <v>0.6013210765859275</v>
+        <v>0.2598889013062394</v>
       </c>
       <c r="C131">
-        <v>0.2015031407353146</v>
+        <v>0.4535732155665912</v>
       </c>
       <c r="D131">
-        <v>0.1971757826787578</v>
+        <v>0.2865378831271693</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>ITC1_Piemonte</t>
-        </is>
-      </c>
-      <c r="B132">
-        <v>0.2592666657302327</v>
+          <t>ITC2_Valle d'Aosta/Vallée d'Aoste</t>
+        </is>
       </c>
       <c r="C132">
-        <v>0.4631682274483765</v>
+        <v>0.4431199397248463</v>
       </c>
       <c r="D132">
-        <v>0.2775651068213908</v>
+        <v>0.5568800602751537</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>ITC2_Valle d'Aosta/Vallée d'Aoste</t>
-        </is>
+          <t>ITC3_Liguria</t>
+        </is>
+      </c>
+      <c r="B133">
+        <v>0.5227812153145973</v>
       </c>
       <c r="C133">
-        <v>0.4446513398102268</v>
+        <v>0.371916339680704</v>
       </c>
       <c r="D133">
-        <v>0.5553486601897732</v>
+        <v>0.1053024450046987</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>ITC3_Liguria</t>
+          <t>ITC4_Lombardia</t>
         </is>
       </c>
       <c r="B134">
-        <v>0.5149070521380731</v>
+        <v>0.4014122209315557</v>
       </c>
       <c r="C134">
-        <v>0.3838085594541467</v>
+        <v>0.5017487729327095</v>
       </c>
       <c r="D134">
-        <v>0.1012843884077803</v>
+        <v>0.09683900613573479</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>ITC4_Lombardia</t>
+          <t>ITF1_Abruzzo</t>
         </is>
       </c>
       <c r="B135">
-        <v>0.4123061655698549</v>
+        <v>0.08378286577942987</v>
       </c>
       <c r="C135">
-        <v>0.4923699959171595</v>
+        <v>0.4735231184059664</v>
       </c>
       <c r="D135">
-        <v>0.09532383851298562</v>
+        <v>0.4426940158146037</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>ITF1_Abruzzo</t>
+          <t>ITF2_Molise</t>
         </is>
       </c>
       <c r="B136">
-        <v>0.1023781904603471</v>
+        <v>0.1809199642254092</v>
       </c>
       <c r="C136">
-        <v>0.4923356833595224</v>
+        <v>0.3071259628055835</v>
       </c>
       <c r="D136">
-        <v>0.4052861261801305</v>
+        <v>0.5119540729690074</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>ITF2_Molise</t>
+          <t>ITF3_Campania</t>
         </is>
       </c>
       <c r="B137">
-        <v>0.1746625868695296</v>
+        <v>0.5513137821497068</v>
       </c>
       <c r="C137">
-        <v>0.3248760788092935</v>
+        <v>0.2901202970888893</v>
       </c>
       <c r="D137">
-        <v>0.500461334321177</v>
+        <v>0.1585659207614039</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>ITF3_Campania</t>
+          <t>ITF4_Puglia</t>
         </is>
       </c>
       <c r="B138">
-        <v>0.5420858615993956</v>
+        <v>0.1986604131251994</v>
       </c>
       <c r="C138">
-        <v>0.2996528258498768</v>
+        <v>0.5147809448334205</v>
       </c>
       <c r="D138">
-        <v>0.1582613125507275</v>
+        <v>0.2865586420413801</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>ITF4_Puglia</t>
+          <t>ITF5_Basilicata</t>
         </is>
       </c>
       <c r="B139">
-        <v>0.2325450721130103</v>
+        <v>0.2377721623404437</v>
       </c>
       <c r="C139">
-        <v>0.5397211995814506</v>
+        <v>0.05926076045924913</v>
       </c>
       <c r="D139">
-        <v>0.2277337283055391</v>
+        <v>0.7029670772003072</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>ITF5_Basilicata</t>
+          <t>ITF6_Calabria</t>
         </is>
       </c>
       <c r="B140">
-        <v>0.2390742957446494</v>
+        <v>0.1560562604558182</v>
       </c>
       <c r="C140">
-        <v>0.1137322194764115</v>
+        <v>0.4657728522644048</v>
       </c>
       <c r="D140">
-        <v>0.6471934847789391</v>
+        <v>0.3781708872797769</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>ITF6_Calabria</t>
+          <t>ITG1_Sicilia</t>
         </is>
       </c>
       <c r="B141">
-        <v>0.1640766713747394</v>
+        <v>0.2821317604666369</v>
       </c>
       <c r="C141">
-        <v>0.4828678741186367</v>
+        <v>0.4923521981513655</v>
       </c>
       <c r="D141">
-        <v>0.3530554545066239</v>
+        <v>0.2255160413819975</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>ITG1_Sicilia</t>
+          <t>ITG2_Sardegna</t>
         </is>
       </c>
       <c r="B142">
-        <v>0.2923470925512478</v>
+        <v>0.1706563197842992</v>
       </c>
       <c r="C142">
-        <v>0.5073149463183204</v>
+        <v>0.3470709002341164</v>
       </c>
       <c r="D142">
-        <v>0.2003379611304318</v>
+        <v>0.4822727799815844</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>ITG2_Sardegna</t>
+          <t>ITH1_Provincia Autonoma di Bolzano/Bozen</t>
         </is>
       </c>
       <c r="B143">
-        <v>0.1631007512933332</v>
+        <v>0.1943508906590245</v>
       </c>
       <c r="C143">
-        <v>0.3857690599599538</v>
+        <v>0.3077280137853424</v>
       </c>
       <c r="D143">
-        <v>0.451130188746713</v>
+        <v>0.4979210955556331</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>ITH1_Provincia Autonoma di Bolzano/Bozen</t>
+          <t>ITH2_Provincia Autonoma di Trento</t>
         </is>
       </c>
       <c r="B144">
-        <v>0.1954931257735795</v>
+        <v>0.2390266658226797</v>
       </c>
       <c r="C144">
-        <v>0.317390438112103</v>
+        <v>0.3692713654056984</v>
       </c>
       <c r="D144">
-        <v>0.4871164361143175</v>
+        <v>0.3917019687716219</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>ITH2_Provincia Autonoma di Trento</t>
+          <t>ITH3_Veneto</t>
         </is>
       </c>
       <c r="B145">
-        <v>0.231379969763357</v>
+        <v>0.1947849298109484</v>
       </c>
       <c r="C145">
-        <v>0.3842900313565384</v>
+        <v>0.6286431013925198</v>
       </c>
       <c r="D145">
-        <v>0.3843299988801047</v>
+        <v>0.1765719687965319</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>ITH3_Veneto</t>
+          <t>ITH4_Friuli-Venezia Giulia</t>
         </is>
       </c>
       <c r="B146">
-        <v>0.1868357294692529</v>
+        <v>0.296802447738261</v>
       </c>
       <c r="C146">
-        <v>0.6457419633823768</v>
+        <v>0.3795049394609918</v>
       </c>
       <c r="D146">
-        <v>0.1674223071483703</v>
+        <v>0.3236926128007472</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>ITH4_Friuli-Venezia Giulia</t>
+          <t>ITH5_Emilia-Romagna</t>
         </is>
       </c>
       <c r="B147">
-        <v>0.294982081917682</v>
+        <v>0.3777283609660368</v>
       </c>
       <c r="C147">
-        <v>0.3852687595186434</v>
+        <v>0.3339421521376452</v>
       </c>
       <c r="D147">
-        <v>0.3197491585636746</v>
+        <v>0.288329486896318</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>ITH5_Emilia-Romagna</t>
+          <t>ITI1_Toscana</t>
         </is>
       </c>
       <c r="B148">
-        <v>0.3818513300625933</v>
+        <v>0.2792639719725697</v>
       </c>
       <c r="C148">
-        <v>0.3595570902244233</v>
+        <v>0.4498139806277149</v>
       </c>
       <c r="D148">
-        <v>0.2585915797129834</v>
+        <v>0.2709220473997154</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>ITI1_Toscana</t>
+          <t>ITI2_Umbria</t>
         </is>
       </c>
       <c r="B149">
-        <v>0.2831461030580059</v>
+        <v>0.3221916494039932</v>
       </c>
       <c r="C149">
-        <v>0.4661636001123881</v>
+        <v>0.2297733916247546</v>
       </c>
       <c r="D149">
-        <v>0.2506902968296061</v>
+        <v>0.4480349589712522</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>ITI2_Umbria</t>
+          <t>ITI3_Marche</t>
         </is>
       </c>
       <c r="B150">
-        <v>0.3211936668266971</v>
+        <v>0.1228400116970297</v>
       </c>
       <c r="C150">
-        <v>0.2675928805739831</v>
+        <v>0.6237499449856942</v>
       </c>
       <c r="D150">
-        <v>0.4112134525993199</v>
+        <v>0.253410043317276</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>ITI3_Marche</t>
+          <t>ITI4_Lazio</t>
         </is>
       </c>
       <c r="B151">
-        <v>0.126858725419368</v>
+        <v>0.5453685643247278</v>
       </c>
       <c r="C151">
-        <v>0.6332577142789755</v>
+        <v>0.2487709066698892</v>
       </c>
       <c r="D151">
-        <v>0.2398835603016566</v>
+        <v>0.2058605290053829</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>ITI4_Lazio</t>
+          <t>LT01_Sostinės regionas</t>
         </is>
       </c>
       <c r="B152">
-        <v>0.546037187996717</v>
+        <v>0.7171858009982419</v>
       </c>
       <c r="C152">
-        <v>0.2756465385948639</v>
+        <v>0.03632575750558573</v>
       </c>
       <c r="D152">
-        <v>0.1783162734084191</v>
+        <v>0.2464884414961724</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>LT01_Sostinės regionas</t>
+          <t>LT02_Vidurio ir vakarų Lietuvos regionas</t>
         </is>
       </c>
       <c r="B153">
-        <v>0.7181341035445891</v>
+        <v>0.3652872036430191</v>
       </c>
       <c r="C153">
-        <v>0.05465424200916244</v>
+        <v>0.1807761445477617</v>
       </c>
       <c r="D153">
-        <v>0.2272116544462485</v>
+        <v>0.4539366518092192</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>LT02_Vidurio ir vakarų Lietuvos regionas</t>
+          <t>LU00_Luxembourg</t>
         </is>
       </c>
       <c r="B154">
-        <v>0.3666489247483849</v>
+        <v>0.2187304360827539</v>
       </c>
       <c r="C154">
-        <v>0.1949936853580391</v>
+        <v>0.4076371988903433</v>
       </c>
       <c r="D154">
-        <v>0.438357389893576</v>
+        <v>0.3736323650269028</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>LU00_Luxembourg</t>
+          <t>LV00_Latvia</t>
         </is>
       </c>
       <c r="B155">
-        <v>0.2221280201963648</v>
+        <v>0.4658677022195122</v>
       </c>
       <c r="C155">
-        <v>0.3975938665807668</v>
+        <v>0.2167564644998129</v>
       </c>
       <c r="D155">
-        <v>0.3802781132228684</v>
+        <v>0.317375833280675</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>LV00_Latvia</t>
+          <t>MT00_Malta</t>
         </is>
       </c>
       <c r="B156">
-        <v>0.4532528009492238</v>
+        <v>0.4895435673721535</v>
       </c>
       <c r="C156">
-        <v>0.2221899880323429</v>
+        <v>0.4812336311905633</v>
       </c>
       <c r="D156">
-        <v>0.3245572110184333</v>
+        <v>0.02922280143728311</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>MT00_Malta</t>
+          <t>NL00_The Netherlands</t>
         </is>
       </c>
       <c r="B157">
-        <v>0.4833706949528338</v>
+        <v>0.5654666691436431</v>
       </c>
       <c r="C157">
-        <v>0.487806128014162</v>
+        <v>0.3306597907065341</v>
       </c>
       <c r="D157">
-        <v>0.02882317703300421</v>
+        <v>0.1038735401498228</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>NL00_The Netherlands</t>
+          <t>PL21_Małopolskie</t>
         </is>
       </c>
       <c r="B158">
-        <v>0.5671473333557793</v>
+        <v>0.3562592637320484</v>
       </c>
       <c r="C158">
-        <v>0.3294872524528846</v>
+        <v>0.2698771971179885</v>
       </c>
       <c r="D158">
-        <v>0.1033654141913361</v>
+        <v>0.3738635391499631</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>PL21_Małopolskie</t>
+          <t>PL22_Śląskie</t>
         </is>
       </c>
       <c r="B159">
-        <v>0.3364643683740443</v>
+        <v>0.5911912504109011</v>
       </c>
       <c r="C159">
-        <v>0.3125504568561631</v>
+        <v>0.2604441045135216</v>
       </c>
       <c r="D159">
-        <v>0.3509851747697926</v>
+        <v>0.1483646450755772</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>PL22_Śląskie</t>
+          <t>PL41_Wielkopolskie</t>
         </is>
       </c>
       <c r="B160">
-        <v>0.5784064160656502</v>
+        <v>0.298941250338791</v>
       </c>
       <c r="C160">
-        <v>0.2739864380211395</v>
+        <v>0.314159815327765</v>
       </c>
       <c r="D160">
-        <v>0.1476071459132103</v>
+        <v>0.3868989343334439</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>PL41_Wielkopolskie</t>
+          <t>PL42_Zachodniopomorskie</t>
         </is>
       </c>
       <c r="B161">
-        <v>0.2848221757757397</v>
+        <v>0.3902351704956694</v>
       </c>
       <c r="C161">
-        <v>0.2996972185207133</v>
+        <v>0.3745472239004611</v>
       </c>
       <c r="D161">
-        <v>0.4154806057035469</v>
+        <v>0.2352176056038695</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>PL42_Zachodniopomorskie</t>
+          <t>PL43_Lubuskie</t>
         </is>
       </c>
       <c r="B162">
-        <v>0.385338316940538</v>
+        <v>0.2968211228826447</v>
       </c>
       <c r="C162">
-        <v>0.3092693624539303</v>
+        <v>0.4168169751869585</v>
       </c>
       <c r="D162">
-        <v>0.3053923206055317</v>
+        <v>0.2863619019303967</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>PL43_Lubuskie</t>
+          <t>PL51_Dolnośląskie</t>
         </is>
       </c>
       <c r="B163">
-        <v>0.29308868703787</v>
+        <v>0.4328767484358544</v>
       </c>
       <c r="C163">
-        <v>0.3674703249996969</v>
+        <v>0.2930188907472645</v>
       </c>
       <c r="D163">
-        <v>0.339440987962433</v>
+        <v>0.2741043608168811</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>PL51_Dolnośląskie</t>
+          <t>PL52_Opolskie</t>
         </is>
       </c>
       <c r="B164">
-        <v>0.4198731520604656</v>
+        <v>0.1531957163772781</v>
       </c>
       <c r="C164">
-        <v>0.2597120117042621</v>
+        <v>0.4580573388898276</v>
       </c>
       <c r="D164">
-        <v>0.3204148362352724</v>
+        <v>0.3887469447328943</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>PL52_Opolskie</t>
+          <t>PL61_Kujawsko-pomorskie</t>
         </is>
       </c>
       <c r="B165">
-        <v>0.1417475854777023</v>
+        <v>0.4194745911772836</v>
       </c>
       <c r="C165">
-        <v>0.4238603777368203</v>
+        <v>0.191801406520003</v>
       </c>
       <c r="D165">
-        <v>0.4343920367854773</v>
+        <v>0.3887240023027134</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>PL61_Kujawsko-pomorskie</t>
+          <t>PL62_Warmińsko-mazurskie</t>
         </is>
       </c>
       <c r="B166">
-        <v>0.4259891343857031</v>
+        <v>0.2862667523730882</v>
       </c>
       <c r="C166">
-        <v>0.1656847114365047</v>
+        <v>0.3198862042550232</v>
       </c>
       <c r="D166">
-        <v>0.4083261541777922</v>
+        <v>0.3938470433718885</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>PL62_Warmińsko-mazurskie</t>
+          <t>PL63_Pomorskie</t>
         </is>
       </c>
       <c r="B167">
-        <v>0.2738178075590688</v>
+        <v>0.3869136734839118</v>
       </c>
       <c r="C167">
-        <v>0.2844881476862056</v>
+        <v>0.2614384351548585</v>
       </c>
       <c r="D167">
-        <v>0.4416940447547256</v>
+        <v>0.3516478913612296</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>PL63_Pomorskie</t>
+          <t>PL71_Łódzkie</t>
         </is>
       </c>
       <c r="B168">
-        <v>0.3854629183481282</v>
+        <v>0.3999795430025412</v>
       </c>
       <c r="C168">
-        <v>0.25330663747395</v>
+        <v>0.2212219233680542</v>
       </c>
       <c r="D168">
-        <v>0.3612304441779218</v>
+        <v>0.3787985336294046</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>PL71_Łódzkie</t>
+          <t>PL72_Świętokrzyskie</t>
         </is>
       </c>
       <c r="B169">
-        <v>0.38250873997826</v>
+        <v>0.2150482826118388</v>
       </c>
       <c r="C169">
-        <v>0.2403125422440481</v>
+        <v>0.219243152537948</v>
       </c>
       <c r="D169">
-        <v>0.3771787177776919</v>
+        <v>0.5657085648502133</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>PL72_Świętokrzyskie</t>
+          <t>PL81_Lubelskie</t>
         </is>
       </c>
       <c r="B170">
-        <v>0.2164263550054412</v>
+        <v>0.2390710376784078</v>
       </c>
       <c r="C170">
-        <v>0.2002761335184237</v>
+        <v>0.2327796133514753</v>
       </c>
       <c r="D170">
-        <v>0.5832975114761352</v>
+        <v>0.5281493489701169</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>PL81_Lubelskie</t>
+          <t>PL82_Podkarpackie</t>
         </is>
       </c>
       <c r="B171">
-        <v>0.2465063734376474</v>
+        <v>0.1848465049888611</v>
       </c>
       <c r="C171">
-        <v>0.2130702947220153</v>
+        <v>0.2524851201930457</v>
       </c>
       <c r="D171">
-        <v>0.5404233318403373</v>
+        <v>0.5626683748180933</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>PL82_Podkarpackie</t>
+          <t>PL84_Podlaskie</t>
         </is>
       </c>
       <c r="B172">
-        <v>0.1752648994182355</v>
+        <v>0.4116280853990318</v>
       </c>
       <c r="C172">
-        <v>0.3002139279524353</v>
+        <v>0.1964955580080021</v>
       </c>
       <c r="D172">
-        <v>0.5245211726293292</v>
+        <v>0.391876356592966</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>PL84_Podlaskie</t>
+          <t>PL91_Warszawski stołeczny</t>
         </is>
       </c>
       <c r="B173">
-        <v>0.4039855242296115</v>
+        <v>0.6241064667713225</v>
       </c>
       <c r="C173">
-        <v>0.1828565794992954</v>
+        <v>0.2262082215080816</v>
       </c>
       <c r="D173">
-        <v>0.4131578962710931</v>
+        <v>0.1496853117205959</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>PL91_Warszawski stołeczny</t>
+          <t>PL92_Mazowiecki regionalny</t>
         </is>
       </c>
       <c r="B174">
-        <v>0.6295400347658993</v>
+        <v>0.183405387534516</v>
       </c>
       <c r="C174">
-        <v>0.2465116365639109</v>
+        <v>0.2833457034066124</v>
       </c>
       <c r="D174">
-        <v>0.1239483286701899</v>
+        <v>0.5332489090588717</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>PL92_Mazowiecki regionalny</t>
+          <t>PT11_Norte</t>
         </is>
       </c>
       <c r="B175">
-        <v>0.16966087168983</v>
+        <v>0.4290296488966042</v>
       </c>
       <c r="C175">
-        <v>0.2746602299169328</v>
+        <v>0.4099223795648102</v>
       </c>
       <c r="D175">
-        <v>0.5556788983932371</v>
+        <v>0.1610479715385856</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>PT11_Norte</t>
+          <t>PT15_Algarve</t>
         </is>
       </c>
       <c r="B176">
-        <v>0.4292803098274127</v>
+        <v>0.1474315857631868</v>
       </c>
       <c r="C176">
-        <v>0.406165048904095</v>
+        <v>0.5659525639208705</v>
       </c>
       <c r="D176">
-        <v>0.1645546412684923</v>
+        <v>0.2866158503159428</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>PT15_Algarve</t>
+          <t>PT16_Centro (PT)</t>
         </is>
       </c>
       <c r="B177">
-        <v>0.1427121793981429</v>
+        <v>0.1585166916375327</v>
       </c>
       <c r="C177">
-        <v>0.5582597184906887</v>
+        <v>0.4232502147955093</v>
       </c>
       <c r="D177">
-        <v>0.2990281021111684</v>
+        <v>0.418233093566958</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>PT16_Centro (PT)</t>
+          <t>PT17_Área Metropolitana de Lisboa</t>
         </is>
       </c>
       <c r="B178">
-        <v>0.1513520744280578</v>
+        <v>0.8799050427847324</v>
       </c>
       <c r="C178">
-        <v>0.4227922335602459</v>
+        <v>0.1083332498555197</v>
       </c>
       <c r="D178">
-        <v>0.4258556920116963</v>
+        <v>0.0117617073597479</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>PT17_Área Metropolitana de Lisboa</t>
-        </is>
-      </c>
-      <c r="B179">
-        <v>0.885085346468917</v>
+          <t>PT18_Alentejo</t>
+        </is>
       </c>
       <c r="C179">
-        <v>0.1045363972062465</v>
+        <v>0.3095536206286908</v>
       </c>
       <c r="D179">
-        <v>0.01037825632483648</v>
+        <v>0.6904463793713091</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>PT18_Alentejo</t>
-        </is>
+          <t>PT20_Região Autónoma dos Açores</t>
+        </is>
+      </c>
+      <c r="B180">
+        <v>0.2806756302850294</v>
       </c>
       <c r="C180">
-        <v>0.3023351207238439</v>
+        <v>0.1882355101092729</v>
       </c>
       <c r="D180">
-        <v>0.6976648792761562</v>
+        <v>0.5310888596056977</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>PT20_Região Autónoma dos Açores</t>
+          <t>PT30_Região Autónoma da Madeira</t>
         </is>
       </c>
       <c r="B181">
-        <v>0.2901643142318934</v>
+        <v>0.3873597110236019</v>
       </c>
       <c r="C181">
-        <v>0.1738051903374323</v>
+        <v>0.4299350997333315</v>
       </c>
       <c r="D181">
-        <v>0.5360304954306744</v>
+        <v>0.1827051892430666</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>PT30_Região Autónoma da Madeira</t>
+          <t>RO11_Nord-Vest</t>
         </is>
       </c>
       <c r="B182">
-        <v>0.3860625737123623</v>
+        <v>0.3378030936855664</v>
       </c>
       <c r="C182">
-        <v>0.426393652880223</v>
+        <v>0.2605127097201722</v>
       </c>
       <c r="D182">
-        <v>0.1875437734074147</v>
+        <v>0.4016841965942614</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>RO11_Nord-Vest</t>
+          <t>RO12_Centru</t>
         </is>
       </c>
       <c r="B183">
-        <v>0.3471182648621047</v>
+        <v>0.3232197699075012</v>
       </c>
       <c r="C183">
-        <v>0.2597985629655537</v>
+        <v>0.3130671796676932</v>
       </c>
       <c r="D183">
-        <v>0.3930831721723416</v>
+        <v>0.3637130504248056</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>RO12_Centru</t>
+          <t>RO21_Nord-Est</t>
         </is>
       </c>
       <c r="B184">
-        <v>0.3233297496000389</v>
+        <v>0.2895470516014307</v>
       </c>
       <c r="C184">
-        <v>0.3104186363899592</v>
+        <v>0.2438947036272048</v>
       </c>
       <c r="D184">
-        <v>0.3662516140100019</v>
+        <v>0.4665582447713646</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>RO21_Nord-Est</t>
+          <t>RO22_Sud-Est</t>
         </is>
       </c>
       <c r="B185">
-        <v>0.2916437556300783</v>
+        <v>0.3670511703215709</v>
       </c>
       <c r="C185">
-        <v>0.2522101312849978</v>
+        <v>0.2661821641491913</v>
       </c>
       <c r="D185">
-        <v>0.4561461130849239</v>
+        <v>0.3667666655292378</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>RO22_Sud-Est</t>
+          <t>RO31_Sud-Muntenia</t>
         </is>
       </c>
       <c r="B186">
-        <v>0.3726417793599271</v>
+        <v>0.2112818781184856</v>
       </c>
       <c r="C186">
-        <v>0.2681845763102756</v>
+        <v>0.3505210777741473</v>
       </c>
       <c r="D186">
-        <v>0.3591736443297973</v>
+        <v>0.4381970441073672</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>RO31_Sud-Muntenia</t>
+          <t>RO32_Bucureşti-Ilfov</t>
         </is>
       </c>
       <c r="B187">
-        <v>0.2187989899338277</v>
+        <v>0.815153375494245</v>
       </c>
       <c r="C187">
-        <v>0.3570261233913743</v>
+        <v>0.1339615421119646</v>
       </c>
       <c r="D187">
-        <v>0.424174886674798</v>
+        <v>0.05088508239379038</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>RO32_Bucureşti-Ilfov</t>
+          <t>RO41_Sud-Vest Oltenia</t>
         </is>
       </c>
       <c r="B188">
-        <v>0.8169447854769608</v>
+        <v>0.3591823211325718</v>
       </c>
       <c r="C188">
-        <v>0.1344811511840423</v>
+        <v>0.2229227467454317</v>
       </c>
       <c r="D188">
-        <v>0.04857406333899682</v>
+        <v>0.4178949321219965</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>RO41_Sud-Vest Oltenia</t>
+          <t>RO42_Vest</t>
         </is>
       </c>
       <c r="B189">
-        <v>0.3660882421990707</v>
+        <v>0.3039682858472263</v>
       </c>
       <c r="C189">
-        <v>0.2245564810113178</v>
+        <v>0.378067733799442</v>
       </c>
       <c r="D189">
-        <v>0.4093552767896114</v>
+        <v>0.3179639803533318</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>RO42_Vest</t>
+          <t>SE11_Stockholm</t>
         </is>
       </c>
       <c r="B190">
-        <v>0.2966240538102212</v>
+        <v>0.6101770999131676</v>
       </c>
       <c r="C190">
-        <v>0.3780642216126256</v>
+        <v>0.3042485853775101</v>
       </c>
       <c r="D190">
-        <v>0.3253117245771532</v>
+        <v>0.08557431470932231</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>SE11_Stockholm</t>
+          <t>SE12_Östra Mellansverige</t>
         </is>
       </c>
       <c r="B191">
-        <v>0.6082665043414508</v>
+        <v>0.5255142467544611</v>
       </c>
       <c r="C191">
-        <v>0.3081685384932941</v>
+        <v>0.2945324404271635</v>
       </c>
       <c r="D191">
-        <v>0.08356495716525514</v>
+        <v>0.1799533128183753</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>SE12_Östra Mellansverige</t>
+          <t>SE21_Småland med öarna</t>
         </is>
       </c>
       <c r="B192">
-        <v>0.5224269877607779</v>
+        <v>0</v>
       </c>
       <c r="C192">
-        <v>0.2930610614449597</v>
+        <v>0.5937525187925523</v>
       </c>
       <c r="D192">
-        <v>0.1845119507942624</v>
+        <v>0.4062474812074477</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>SE21_Småland med öarna</t>
+          <t>SE22_Sydsverige</t>
         </is>
       </c>
       <c r="B193">
-        <v>0</v>
+        <v>0.4296920566558973</v>
       </c>
       <c r="C193">
-        <v>0.5914187533915242</v>
+        <v>0.2026784334088619</v>
       </c>
       <c r="D193">
-        <v>0.4085812466084758</v>
+        <v>0.3676295099352409</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>SE22_Sydsverige</t>
+          <t>SE23_Västsverige</t>
         </is>
       </c>
       <c r="B194">
-        <v>0.429616137138159</v>
+        <v>0.3106765298124246</v>
       </c>
       <c r="C194">
-        <v>0.196457293119205</v>
+        <v>0.3647421043876915</v>
       </c>
       <c r="D194">
-        <v>0.373926569742636</v>
+        <v>0.3245813657998839</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>SE23_Västsverige</t>
+          <t>SE31_Norra Mellansverige</t>
         </is>
       </c>
       <c r="B195">
-        <v>0.3122085523535871</v>
+        <v>0</v>
       </c>
       <c r="C195">
-        <v>0.3704458733720802</v>
+        <v>0.5450503873481624</v>
       </c>
       <c r="D195">
-        <v>0.3173455742743326</v>
+        <v>0.4549496126518376</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>SE31_Norra Mellansverige</t>
+          <t>SE32_Mellersta Norrland</t>
         </is>
       </c>
       <c r="B196">
         <v>0</v>
       </c>
       <c r="C196">
-        <v>0.5546925505148248</v>
+        <v>0.6012486965557851</v>
       </c>
       <c r="D196">
-        <v>0.4453074494851753</v>
+        <v>0.3987513034442149</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>SE32_Mellersta Norrland</t>
+          <t>SE33_Övre Norrland</t>
         </is>
       </c>
       <c r="B197">
-        <v>0</v>
+        <v>0.2682859818622558</v>
       </c>
       <c r="C197">
-        <v>0.5833143381303761</v>
+        <v>0.4020185016186696</v>
       </c>
       <c r="D197">
-        <v>0.4166856618696239</v>
+        <v>0.3296955165190745</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>SE33_Övre Norrland</t>
+          <t>SI03_Vzhodna Slovenija</t>
         </is>
       </c>
       <c r="B198">
-        <v>0.2673224213305354</v>
+        <v>0.1058716877939524</v>
       </c>
       <c r="C198">
-        <v>0.4121447255620595</v>
+        <v>0.2718723413315356</v>
       </c>
       <c r="D198">
-        <v>0.3205328531074051</v>
+        <v>0.622255970874512</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>SI03_Vzhodna Slovenija</t>
+          <t>SI04_Zahodna Slovenija</t>
         </is>
       </c>
       <c r="B199">
-        <v>0.1016341808479081</v>
+        <v>0.2991979772642557</v>
       </c>
       <c r="C199">
-        <v>0.2768046458768605</v>
+        <v>0.4419277801961493</v>
       </c>
       <c r="D199">
-        <v>0.6215611732752314</v>
+        <v>0.2588742425395951</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>SI04_Zahodna Slovenija</t>
+          <t>SK01_Bratislavský kraj</t>
         </is>
       </c>
       <c r="B200">
-        <v>0.3009266085897054</v>
+        <v>0.6365727388488343</v>
       </c>
       <c r="C200">
-        <v>0.4353694377106486</v>
+        <v>0.1624248931939551</v>
       </c>
       <c r="D200">
-        <v>0.263703953699646</v>
+        <v>0.2010023679572106</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>SK01_Bratislavský kraj</t>
+          <t>SK02_Západné Slovensko</t>
         </is>
       </c>
       <c r="B201">
-        <v>0.6355647369954284</v>
+        <v>0.1314583708720466</v>
       </c>
       <c r="C201">
-        <v>0.1848034906276039</v>
+        <v>0.428378744133823</v>
       </c>
       <c r="D201">
-        <v>0.1796317723769677</v>
+        <v>0.4401628849941303</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>SK02_Západné Slovensko</t>
+          <t>SK03_Stredné Slovensko</t>
         </is>
       </c>
       <c r="B202">
-        <v>0.1188139890183127</v>
+        <v>0.1436438954659409</v>
       </c>
       <c r="C202">
-        <v>0.4197924733157075</v>
+        <v>0.408667618345023</v>
       </c>
       <c r="D202">
-        <v>0.4613935376659798</v>
+        <v>0.4476884861890361</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>SK03_Stredné Slovensko</t>
+          <t>SK04_Východné Slovensko</t>
         </is>
       </c>
       <c r="B203">
-        <v>0.1424257330288101</v>
+        <v>0.2001451161137872</v>
       </c>
       <c r="C203">
-        <v>0.4377224031867911</v>
+        <v>0.3373831499768558</v>
       </c>
       <c r="D203">
-        <v>0.4198518637843988</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>SK04_Východné Slovensko</t>
-        </is>
-      </c>
-      <c r="B204">
-        <v>0.2062955619557333</v>
-      </c>
-      <c r="C204">
-        <v>0.3439403615834961</v>
-      </c>
-      <c r="D204">
-        <v>0.4497640764607707</v>
+        <v>0.462471733909357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>